<commit_message>
change style for week headers
</commit_message>
<xml_diff>
--- a/tests/5782 Regular.xlsx
+++ b/tests/5782 Regular.xlsx
@@ -8634,7 +8634,7 @@
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="1:14" ht="12" customHeight="1">
+    <row r="3" spans="1:14" ht="12.3" customHeight="1">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -11986,7 +11986,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="88" spans="1:14" ht="12" customHeight="1">
+    <row r="88" spans="1:14" ht="12.3" customHeight="1">
       <c r="A88" s="4" t="s">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
fixing week header styling
</commit_message>
<xml_diff>
--- a/tests/5782 Regular.xlsx
+++ b/tests/5782 Regular.xlsx
@@ -8522,11 +8522,11 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf applyFont="1" fontId="1" applyAlignment="1">
-      <alignment/>
+      <alignment vertical="center"/>
     </xf>
     <xf applyFont="1" fontId="0" applyBorder="1" borderId="1"/>
     <xf applyFont="1" fontId="1" applyBorder="1" borderId="1" applyAlignment="1">
-      <alignment/>
+      <alignment vertical="center"/>
     </xf>
     <xf applyFont="1" fontId="2"/>
     <xf applyFont="1" fontId="1"/>

</xml_diff>